<commit_message>
Updated regional staff salary computation
</commit_message>
<xml_diff>
--- a/model_inputs/labour_reports/staff_salaries.xlsx
+++ b/model_inputs/labour_reports/staff_salaries.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjc92\Downloads\LMBME Service Delivery Cost Model\model_inputs\labour_reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjc92\Downloads\biomed-service-delivery-cost-model\model_inputs\labour_reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3145F1B4-64FE-4562-AA2E-DC7129968A97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F866B162-3A6F-4828-A7C3-2A80E75CE9D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1086,7 +1086,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,8 +1801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726CAD88-95B2-48F4-83A5-5059E9D62D0D}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2870,15 +2870,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FF89A6-1CD6-4DA3-AA16-6BCC8BA59369}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -3150,6 +3150,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008B72074D08840F4A907EA3B37AB4414E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7356207cb152440f28e0cdf491afbdb0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -3263,33 +3278,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D72C636-6F61-4865-A889-4D5549F92FE9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED56B025-4D52-411E-B5B1-9A793E8274FF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3310,9 +3302,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED56B025-4D52-411E-B5B1-9A793E8274FF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D72C636-6F61-4865-A889-4D5549F92FE9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>